<commit_message>
Update report and presentation
</commit_message>
<xml_diff>
--- a/Results/Summary.xlsx
+++ b/Results/Summary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Roy Hachnochi\Documents\Masters\Digital Signal Processing\Project\Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8184F9B6-995A-4451-BF94-C2E430E3B536}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82EBC196-4954-4321-A20C-229F935131CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -88,13 +88,19 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="20">
     <border>
@@ -325,7 +331,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -408,6 +414,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -417,25 +438,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -755,7 +764,7 @@
   <dimension ref="A1:F49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="E6" sqref="A1:F49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -769,30 +778,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15" thickBot="1">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="37" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="36" t="s">
+      <c r="F1" s="38" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="28">
+      <c r="A2" s="33">
         <v>10</v>
       </c>
-      <c r="B2" s="31" t="s">
+      <c r="B2" s="32" t="s">
         <v>4</v>
       </c>
       <c r="C2" s="7" t="s">
@@ -809,8 +818,8 @@
       </c>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="29"/>
-      <c r="B3" s="32"/>
+      <c r="A3" s="34"/>
+      <c r="B3" s="30"/>
       <c r="C3" s="3" t="s">
         <v>2</v>
       </c>
@@ -825,9 +834,9 @@
       </c>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="29"/>
-      <c r="B4" s="33"/>
-      <c r="C4" s="37" t="s">
+      <c r="A4" s="34"/>
+      <c r="B4" s="31"/>
+      <c r="C4" s="28" t="s">
         <v>3</v>
       </c>
       <c r="D4" s="12">
@@ -841,8 +850,8 @@
       </c>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="29"/>
-      <c r="B5" s="34" t="s">
+      <c r="A5" s="34"/>
+      <c r="B5" s="29" t="s">
         <v>5</v>
       </c>
       <c r="C5" s="3" t="s">
@@ -859,8 +868,8 @@
       </c>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="29"/>
-      <c r="B6" s="32"/>
+      <c r="A6" s="34"/>
+      <c r="B6" s="30"/>
       <c r="C6" s="3" t="s">
         <v>2</v>
       </c>
@@ -875,9 +884,9 @@
       </c>
     </row>
     <row r="7" spans="1:6">
-      <c r="A7" s="29"/>
-      <c r="B7" s="33"/>
-      <c r="C7" s="37" t="s">
+      <c r="A7" s="34"/>
+      <c r="B7" s="31"/>
+      <c r="C7" s="28" t="s">
         <v>3</v>
       </c>
       <c r="D7" s="12">
@@ -891,8 +900,8 @@
       </c>
     </row>
     <row r="8" spans="1:6">
-      <c r="A8" s="29"/>
-      <c r="B8" s="34" t="s">
+      <c r="A8" s="34"/>
+      <c r="B8" s="29" t="s">
         <v>6</v>
       </c>
       <c r="C8" s="3" t="s">
@@ -909,8 +918,8 @@
       </c>
     </row>
     <row r="9" spans="1:6">
-      <c r="A9" s="29"/>
-      <c r="B9" s="32"/>
+      <c r="A9" s="34"/>
+      <c r="B9" s="30"/>
       <c r="C9" s="3" t="s">
         <v>2</v>
       </c>
@@ -925,9 +934,9 @@
       </c>
     </row>
     <row r="10" spans="1:6">
-      <c r="A10" s="29"/>
-      <c r="B10" s="33"/>
-      <c r="C10" s="37" t="s">
+      <c r="A10" s="34"/>
+      <c r="B10" s="31"/>
+      <c r="C10" s="28" t="s">
         <v>3</v>
       </c>
       <c r="D10" s="12">
@@ -941,8 +950,8 @@
       </c>
     </row>
     <row r="11" spans="1:6">
-      <c r="A11" s="29"/>
-      <c r="B11" s="34" t="s">
+      <c r="A11" s="34"/>
+      <c r="B11" s="29" t="s">
         <v>7</v>
       </c>
       <c r="C11" s="3" t="s">
@@ -959,8 +968,8 @@
       </c>
     </row>
     <row r="12" spans="1:6">
-      <c r="A12" s="29"/>
-      <c r="B12" s="32"/>
+      <c r="A12" s="34"/>
+      <c r="B12" s="30"/>
       <c r="C12" s="3" t="s">
         <v>2</v>
       </c>
@@ -975,9 +984,9 @@
       </c>
     </row>
     <row r="13" spans="1:6">
-      <c r="A13" s="29"/>
-      <c r="B13" s="33"/>
-      <c r="C13" s="37" t="s">
+      <c r="A13" s="34"/>
+      <c r="B13" s="31"/>
+      <c r="C13" s="28" t="s">
         <v>3</v>
       </c>
       <c r="D13" s="12">
@@ -991,8 +1000,8 @@
       </c>
     </row>
     <row r="14" spans="1:6">
-      <c r="A14" s="29"/>
-      <c r="B14" s="34" t="s">
+      <c r="A14" s="34"/>
+      <c r="B14" s="29" t="s">
         <v>8</v>
       </c>
       <c r="C14" s="3" t="s">
@@ -1009,8 +1018,8 @@
       </c>
     </row>
     <row r="15" spans="1:6">
-      <c r="A15" s="29"/>
-      <c r="B15" s="32"/>
+      <c r="A15" s="34"/>
+      <c r="B15" s="30"/>
       <c r="C15" s="3" t="s">
         <v>2</v>
       </c>
@@ -1025,9 +1034,9 @@
       </c>
     </row>
     <row r="16" spans="1:6">
-      <c r="A16" s="29"/>
-      <c r="B16" s="33"/>
-      <c r="C16" s="37" t="s">
+      <c r="A16" s="34"/>
+      <c r="B16" s="31"/>
+      <c r="C16" s="28" t="s">
         <v>3</v>
       </c>
       <c r="D16" s="12">
@@ -1041,7 +1050,7 @@
       </c>
     </row>
     <row r="17" spans="1:6" ht="15" thickBot="1">
-      <c r="A17" s="30"/>
+      <c r="A17" s="35"/>
       <c r="B17" s="6" t="s">
         <v>9</v>
       </c>
@@ -1059,10 +1068,10 @@
       </c>
     </row>
     <row r="18" spans="1:6">
-      <c r="A18" s="28">
+      <c r="A18" s="33">
         <v>20</v>
       </c>
-      <c r="B18" s="31" t="s">
+      <c r="B18" s="32" t="s">
         <v>4</v>
       </c>
       <c r="C18" s="7" t="s">
@@ -1079,8 +1088,8 @@
       </c>
     </row>
     <row r="19" spans="1:6">
-      <c r="A19" s="29"/>
-      <c r="B19" s="32"/>
+      <c r="A19" s="34"/>
+      <c r="B19" s="30"/>
       <c r="C19" s="3" t="s">
         <v>2</v>
       </c>
@@ -1095,9 +1104,9 @@
       </c>
     </row>
     <row r="20" spans="1:6">
-      <c r="A20" s="29"/>
-      <c r="B20" s="33"/>
-      <c r="C20" s="37" t="s">
+      <c r="A20" s="34"/>
+      <c r="B20" s="31"/>
+      <c r="C20" s="28" t="s">
         <v>3</v>
       </c>
       <c r="D20" s="16">
@@ -1111,8 +1120,8 @@
       </c>
     </row>
     <row r="21" spans="1:6">
-      <c r="A21" s="29"/>
-      <c r="B21" s="34" t="s">
+      <c r="A21" s="34"/>
+      <c r="B21" s="29" t="s">
         <v>5</v>
       </c>
       <c r="C21" s="3" t="s">
@@ -1129,8 +1138,8 @@
       </c>
     </row>
     <row r="22" spans="1:6">
-      <c r="A22" s="29"/>
-      <c r="B22" s="32"/>
+      <c r="A22" s="34"/>
+      <c r="B22" s="30"/>
       <c r="C22" s="3" t="s">
         <v>2</v>
       </c>
@@ -1145,9 +1154,9 @@
       </c>
     </row>
     <row r="23" spans="1:6">
-      <c r="A23" s="29"/>
-      <c r="B23" s="33"/>
-      <c r="C23" s="37" t="s">
+      <c r="A23" s="34"/>
+      <c r="B23" s="31"/>
+      <c r="C23" s="28" t="s">
         <v>3</v>
       </c>
       <c r="D23" s="16">
@@ -1161,8 +1170,8 @@
       </c>
     </row>
     <row r="24" spans="1:6">
-      <c r="A24" s="29"/>
-      <c r="B24" s="34" t="s">
+      <c r="A24" s="34"/>
+      <c r="B24" s="29" t="s">
         <v>6</v>
       </c>
       <c r="C24" s="3" t="s">
@@ -1179,8 +1188,8 @@
       </c>
     </row>
     <row r="25" spans="1:6">
-      <c r="A25" s="29"/>
-      <c r="B25" s="32"/>
+      <c r="A25" s="34"/>
+      <c r="B25" s="30"/>
       <c r="C25" s="3" t="s">
         <v>2</v>
       </c>
@@ -1195,9 +1204,9 @@
       </c>
     </row>
     <row r="26" spans="1:6">
-      <c r="A26" s="29"/>
-      <c r="B26" s="33"/>
-      <c r="C26" s="37" t="s">
+      <c r="A26" s="34"/>
+      <c r="B26" s="31"/>
+      <c r="C26" s="28" t="s">
         <v>3</v>
       </c>
       <c r="D26" s="12">
@@ -1211,8 +1220,8 @@
       </c>
     </row>
     <row r="27" spans="1:6">
-      <c r="A27" s="29"/>
-      <c r="B27" s="34" t="s">
+      <c r="A27" s="34"/>
+      <c r="B27" s="29" t="s">
         <v>7</v>
       </c>
       <c r="C27" s="3" t="s">
@@ -1229,8 +1238,8 @@
       </c>
     </row>
     <row r="28" spans="1:6">
-      <c r="A28" s="29"/>
-      <c r="B28" s="32"/>
+      <c r="A28" s="34"/>
+      <c r="B28" s="30"/>
       <c r="C28" s="3" t="s">
         <v>2</v>
       </c>
@@ -1245,9 +1254,9 @@
       </c>
     </row>
     <row r="29" spans="1:6">
-      <c r="A29" s="29"/>
-      <c r="B29" s="33"/>
-      <c r="C29" s="37" t="s">
+      <c r="A29" s="34"/>
+      <c r="B29" s="31"/>
+      <c r="C29" s="28" t="s">
         <v>3</v>
       </c>
       <c r="D29" s="16">
@@ -1261,8 +1270,8 @@
       </c>
     </row>
     <row r="30" spans="1:6">
-      <c r="A30" s="29"/>
-      <c r="B30" s="34" t="s">
+      <c r="A30" s="34"/>
+      <c r="B30" s="29" t="s">
         <v>8</v>
       </c>
       <c r="C30" s="3" t="s">
@@ -1279,8 +1288,8 @@
       </c>
     </row>
     <row r="31" spans="1:6">
-      <c r="A31" s="29"/>
-      <c r="B31" s="32"/>
+      <c r="A31" s="34"/>
+      <c r="B31" s="30"/>
       <c r="C31" s="3" t="s">
         <v>2</v>
       </c>
@@ -1295,9 +1304,9 @@
       </c>
     </row>
     <row r="32" spans="1:6">
-      <c r="A32" s="29"/>
-      <c r="B32" s="33"/>
-      <c r="C32" s="37" t="s">
+      <c r="A32" s="34"/>
+      <c r="B32" s="31"/>
+      <c r="C32" s="28" t="s">
         <v>3</v>
       </c>
       <c r="D32" s="12">
@@ -1311,7 +1320,7 @@
       </c>
     </row>
     <row r="33" spans="1:6" ht="15" thickBot="1">
-      <c r="A33" s="30"/>
+      <c r="A33" s="35"/>
       <c r="B33" s="6" t="s">
         <v>9</v>
       </c>
@@ -1329,10 +1338,10 @@
       </c>
     </row>
     <row r="34" spans="1:6">
-      <c r="A34" s="28">
+      <c r="A34" s="33">
         <v>30</v>
       </c>
-      <c r="B34" s="31" t="s">
+      <c r="B34" s="32" t="s">
         <v>4</v>
       </c>
       <c r="C34" s="3" t="s">
@@ -1349,8 +1358,8 @@
       </c>
     </row>
     <row r="35" spans="1:6">
-      <c r="A35" s="29"/>
-      <c r="B35" s="32"/>
+      <c r="A35" s="34"/>
+      <c r="B35" s="30"/>
       <c r="C35" s="3" t="s">
         <v>2</v>
       </c>
@@ -1365,9 +1374,9 @@
       </c>
     </row>
     <row r="36" spans="1:6">
-      <c r="A36" s="29"/>
-      <c r="B36" s="33"/>
-      <c r="C36" s="37" t="s">
+      <c r="A36" s="34"/>
+      <c r="B36" s="31"/>
+      <c r="C36" s="28" t="s">
         <v>3</v>
       </c>
       <c r="D36" s="16">
@@ -1381,8 +1390,8 @@
       </c>
     </row>
     <row r="37" spans="1:6">
-      <c r="A37" s="29"/>
-      <c r="B37" s="34" t="s">
+      <c r="A37" s="34"/>
+      <c r="B37" s="29" t="s">
         <v>5</v>
       </c>
       <c r="C37" s="3" t="s">
@@ -1399,8 +1408,8 @@
       </c>
     </row>
     <row r="38" spans="1:6">
-      <c r="A38" s="29"/>
-      <c r="B38" s="32"/>
+      <c r="A38" s="34"/>
+      <c r="B38" s="30"/>
       <c r="C38" s="3" t="s">
         <v>2</v>
       </c>
@@ -1415,9 +1424,9 @@
       </c>
     </row>
     <row r="39" spans="1:6">
-      <c r="A39" s="29"/>
-      <c r="B39" s="33"/>
-      <c r="C39" s="37" t="s">
+      <c r="A39" s="34"/>
+      <c r="B39" s="31"/>
+      <c r="C39" s="28" t="s">
         <v>3</v>
       </c>
       <c r="D39" s="16">
@@ -1431,8 +1440,8 @@
       </c>
     </row>
     <row r="40" spans="1:6">
-      <c r="A40" s="29"/>
-      <c r="B40" s="34" t="s">
+      <c r="A40" s="34"/>
+      <c r="B40" s="29" t="s">
         <v>6</v>
       </c>
       <c r="C40" s="3" t="s">
@@ -1449,8 +1458,8 @@
       </c>
     </row>
     <row r="41" spans="1:6">
-      <c r="A41" s="29"/>
-      <c r="B41" s="32"/>
+      <c r="A41" s="34"/>
+      <c r="B41" s="30"/>
       <c r="C41" s="3" t="s">
         <v>2</v>
       </c>
@@ -1465,9 +1474,9 @@
       </c>
     </row>
     <row r="42" spans="1:6">
-      <c r="A42" s="29"/>
-      <c r="B42" s="33"/>
-      <c r="C42" s="37" t="s">
+      <c r="A42" s="34"/>
+      <c r="B42" s="31"/>
+      <c r="C42" s="28" t="s">
         <v>3</v>
       </c>
       <c r="D42" s="16">
@@ -1481,8 +1490,8 @@
       </c>
     </row>
     <row r="43" spans="1:6">
-      <c r="A43" s="29"/>
-      <c r="B43" s="34" t="s">
+      <c r="A43" s="34"/>
+      <c r="B43" s="29" t="s">
         <v>7</v>
       </c>
       <c r="C43" s="3" t="s">
@@ -1499,8 +1508,8 @@
       </c>
     </row>
     <row r="44" spans="1:6">
-      <c r="A44" s="29"/>
-      <c r="B44" s="32"/>
+      <c r="A44" s="34"/>
+      <c r="B44" s="30"/>
       <c r="C44" s="3" t="s">
         <v>2</v>
       </c>
@@ -1515,9 +1524,9 @@
       </c>
     </row>
     <row r="45" spans="1:6">
-      <c r="A45" s="29"/>
-      <c r="B45" s="33"/>
-      <c r="C45" s="37" t="s">
+      <c r="A45" s="34"/>
+      <c r="B45" s="31"/>
+      <c r="C45" s="28" t="s">
         <v>3</v>
       </c>
       <c r="D45" s="16">
@@ -1531,8 +1540,8 @@
       </c>
     </row>
     <row r="46" spans="1:6">
-      <c r="A46" s="29"/>
-      <c r="B46" s="34" t="s">
+      <c r="A46" s="34"/>
+      <c r="B46" s="29" t="s">
         <v>8</v>
       </c>
       <c r="C46" s="3" t="s">
@@ -1549,8 +1558,8 @@
       </c>
     </row>
     <row r="47" spans="1:6">
-      <c r="A47" s="29"/>
-      <c r="B47" s="32"/>
+      <c r="A47" s="34"/>
+      <c r="B47" s="30"/>
       <c r="C47" s="3" t="s">
         <v>2</v>
       </c>
@@ -1565,9 +1574,9 @@
       </c>
     </row>
     <row r="48" spans="1:6">
-      <c r="A48" s="29"/>
-      <c r="B48" s="33"/>
-      <c r="C48" s="37" t="s">
+      <c r="A48" s="34"/>
+      <c r="B48" s="31"/>
+      <c r="C48" s="28" t="s">
         <v>3</v>
       </c>
       <c r="D48" s="12">
@@ -1581,7 +1590,7 @@
       </c>
     </row>
     <row r="49" spans="1:6" ht="15" thickBot="1">
-      <c r="A49" s="30"/>
+      <c r="A49" s="35"/>
       <c r="B49" s="6" t="s">
         <v>9</v>
       </c>
@@ -1600,14 +1609,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="B5:B7"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="B24:B26"/>
-    <mergeCell ref="B21:B23"/>
-    <mergeCell ref="B18:B20"/>
-    <mergeCell ref="B14:B16"/>
-    <mergeCell ref="B11:B13"/>
-    <mergeCell ref="B8:B10"/>
     <mergeCell ref="A2:A17"/>
     <mergeCell ref="A18:A33"/>
     <mergeCell ref="A34:A49"/>
@@ -1618,6 +1619,14 @@
     <mergeCell ref="B34:B36"/>
     <mergeCell ref="B30:B32"/>
     <mergeCell ref="B27:B29"/>
+    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="B24:B26"/>
+    <mergeCell ref="B21:B23"/>
+    <mergeCell ref="B18:B20"/>
+    <mergeCell ref="B14:B16"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="B8:B10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>